<commit_message>
Composter now drops biomass
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/nutrition.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/nutrition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E271EE67-0E8C-2543-A2EE-5794CCD16F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EEB3F3-6C98-024B-8B34-DD0F709D9897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{E04DA74A-E851-4A2B-AFF2-C4A335E1AD4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="216">
   <si>
     <t>supplementaries:pancake</t>
   </si>
@@ -691,6 +691,12 @@
   </si>
   <si>
     <t>frostedheart:cooked_squid_tentacles</t>
+  </si>
+  <si>
+    <t>frostedheart:raw_whale_meat</t>
+  </si>
+  <si>
+    <t>frostedheart:cooked_whale_meat</t>
   </si>
 </sst>
 </file>
@@ -802,7 +808,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
+        <name val="宋体"/>
+        <charset val="254"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1122,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9449E8F2-0FFB-4699-9EC1-364C1E3FECDC}">
-  <dimension ref="A1:O203"/>
+  <dimension ref="A1:O205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="177" zoomScaleNormal="121" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200"/>
+    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="138" zoomScaleNormal="177" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -10091,10 +10121,10 @@
         <v>0</v>
       </c>
       <c r="E180">
-        <v>0</v>
+        <v>1.1857359848670907E-3</v>
       </c>
       <c r="F180">
-        <v>1.1857359848670907E-3</v>
+        <v>0</v>
       </c>
       <c r="G180">
         <v>0</v>
@@ -10112,11 +10142,11 @@
       </c>
       <c r="L180" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.29643399621677269</v>
       </c>
       <c r="M180" s="8">
         <f t="shared" si="17"/>
-        <v>0.29643399621677269</v>
+        <v>0</v>
       </c>
       <c r="N180" s="8">
         <f t="shared" si="18"/>
@@ -11053,27 +11083,27 @@
         <v>4.5197121304413671E-4</v>
       </c>
       <c r="J199" s="8">
-        <f t="shared" ref="J199:J203" si="38">C199*10000/40</f>
+        <f t="shared" ref="J199:J204" si="38">C199*10000/40</f>
         <v>0</v>
       </c>
       <c r="K199" s="8">
-        <f t="shared" ref="K199:K203" si="39">D199*10000/40</f>
+        <f t="shared" ref="K199:K204" si="39">D199*10000/40</f>
         <v>0</v>
       </c>
       <c r="L199" s="8">
-        <f t="shared" ref="L199:L203" si="40">E199*10000/40</f>
+        <f t="shared" ref="L199:L204" si="40">E199*10000/40</f>
         <v>0</v>
       </c>
       <c r="M199" s="8">
-        <f t="shared" ref="M199:M203" si="41">F199*10000/40</f>
+        <f t="shared" ref="M199:M204" si="41">F199*10000/40</f>
         <v>0.11002436832322082</v>
       </c>
       <c r="N199" s="8">
-        <f t="shared" ref="N199:N203" si="42">G199*10000/40</f>
+        <f t="shared" ref="N199:N204" si="42">G199*10000/40</f>
         <v>0</v>
       </c>
       <c r="O199" s="8">
-        <f t="shared" ref="O199:O203" si="43">H199*10000/40</f>
+        <f t="shared" ref="O199:O204" si="43">H199*10000/40</f>
         <v>0.11299280326103418</v>
       </c>
     </row>
@@ -11274,6 +11304,106 @@
       </c>
       <c r="O203" s="8">
         <f t="shared" si="43"/>
+        <v>0.30692740078561104</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15">
+      <c r="A204" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B204" s="3">
+        <v>1</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>4.4009747329288332E-4</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>4.5197121304413671E-4</v>
+      </c>
+      <c r="J204" s="8">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="K204" s="8">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="L204" s="8">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="M204" s="8">
+        <f t="shared" si="41"/>
+        <v>0.11002436832322082</v>
+      </c>
+      <c r="N204" s="8">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="O204" s="8">
+        <f t="shared" si="43"/>
+        <v>0.11299280326103418</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15">
+      <c r="A205" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B205" s="3">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205">
+        <v>1.7786039773006359E-3</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>1.2277096031424442E-3</v>
+      </c>
+      <c r="J205" s="8">
+        <f t="shared" ref="J205" si="44">C205*10000/40</f>
+        <v>0</v>
+      </c>
+      <c r="K205" s="8">
+        <f t="shared" ref="K205" si="45">D205*10000/40</f>
+        <v>0</v>
+      </c>
+      <c r="L205" s="8">
+        <f t="shared" ref="L205" si="46">E205*10000/40</f>
+        <v>0</v>
+      </c>
+      <c r="M205" s="8">
+        <f t="shared" ref="M205" si="47">F205*10000/40</f>
+        <v>0.44465099432515898</v>
+      </c>
+      <c r="N205" s="8">
+        <f t="shared" ref="N205" si="48">G205*10000/40</f>
+        <v>0</v>
+      </c>
+      <c r="O205" s="8">
+        <f t="shared" ref="O205" si="49">H205*10000/40</f>
         <v>0.30692740078561104</v>
       </c>
     </row>
@@ -11284,13 +11414,16 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A192 A200:A65503">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:A192 A200:A203 A205:A65503">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(COUNTIF($A$196:$A$65503, A1)+COUNTIF($A$1:$A$192, A1)&gt;1,NOT(ISBLANK(A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A193:A199">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A204">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>